<commit_message>
Version 2 : add 3 digital I/Os D10, D11, D12. New addresse bit D13, default add 0x58
</commit_message>
<xml_diff>
--- a/02-realisation/04-test/annalogRead190105_0114.xlsx
+++ b/02-realisation/04-test/annalogRead190105_0114.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MountWD\Donnees\OneDrive\Donnees\008_iao_wrk\VoRoboticsAsso\00-ProjetsPerso\050-nanoI2CSlaveExpander\projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MountWD\Donnees\OneDrive\Donnees\008_iao_wrk\VoRoboticsAsso\00-ProjetsPerso\050-nanoI2CSlaveExpander\projet\02-realisation\04-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{C60C5A37-A7AA-47EF-B36C-CFE6EE70F260}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053C986A-F23D-4743-8D52-AE0D62B174AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13335" windowHeight="7680" xr2:uid="{D3FC6CB6-8A89-4399-A90B-A15A1C8E2EBA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" xr2:uid="{D3FC6CB6-8A89-4399-A90B-A15A1C8E2EBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>real</t>
   </si>
   <si>
-    <t>err</t>
+    <t>err %</t>
   </si>
 </sst>
 </file>
@@ -47,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -81,7 +81,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C5B19F-4A55-4922-9AE0-3A663DB3E32E}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>